<commit_message>
ADD: add language info of column when term_expansion and revise
</commit_message>
<xml_diff>
--- a/training/amazon/dbInfo/metadata.xlsx
+++ b/training/amazon/dbInfo/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\something\zebura\training\amazon\dbInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A33154E-0905-4DBF-9B1C-8D00FDFD628E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0925DB1-09CD-4F21-9B9A-DD5EBAFFED45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t>no</t>
   </si>
@@ -292,17 +292,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>#VIRTUAL_IN(product_name)</t>
-  </si>
-  <si>
-    <t>#VIRTUAL_IN(product_name)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>#VIRTUAL_IN(category)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>A name or symbol used to identify a product or company.</t>
   </si>
   <si>
@@ -323,6 +312,22 @@
   </si>
   <si>
     <t>context; case</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>English</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIRTUAL_IN(category.%{value}%)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIRTUAL_IN(product_name.%{value}%)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1405,7 +1410,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1"/>
@@ -1415,7 +1420,7 @@
     <col min="12" max="13" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.25" customHeight="1">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1452,8 +1457,11 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="20.25" customHeight="1">
       <c r="B2" t="s">
         <v>69</v>
       </c>
@@ -1464,7 +1472,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1">
+    <row r="3" spans="1:13" ht="20.25" customHeight="1">
       <c r="C3" t="s">
         <v>21</v>
       </c>
@@ -1481,7 +1489,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1">
+    <row r="4" spans="1:13" ht="20.25" customHeight="1">
       <c r="C4" t="s">
         <v>10</v>
       </c>
@@ -1494,8 +1502,11 @@
       <c r="J4" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="20.25" customHeight="1">
       <c r="C5" t="s">
         <v>22</v>
       </c>
@@ -1508,8 +1519,11 @@
       <c r="J5" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="20.25" customHeight="1">
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1523,7 +1537,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="20.25" customHeight="1">
+    <row r="7" spans="1:13" ht="20.25" customHeight="1">
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1537,7 +1551,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1">
+    <row r="8" spans="1:13" ht="20.25" customHeight="1">
       <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1551,7 +1565,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="20.25" customHeight="1">
+    <row r="9" spans="1:13" ht="20.25" customHeight="1">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -1565,7 +1579,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.25" customHeight="1">
+    <row r="10" spans="1:13" ht="20.25" customHeight="1">
       <c r="C10" t="s">
         <v>27</v>
       </c>
@@ -1580,7 +1594,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:12" ht="20.25" customHeight="1">
+    <row r="11" spans="1:13" ht="20.25" customHeight="1">
       <c r="C11" t="s">
         <v>28</v>
       </c>
@@ -1594,8 +1608,11 @@
         <v>75</v>
       </c>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.25" customHeight="1">
       <c r="C12" t="s">
         <v>29</v>
       </c>
@@ -1610,7 +1627,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:12" ht="20.25" customHeight="1">
+    <row r="13" spans="1:13" ht="20.25" customHeight="1">
       <c r="C13" t="s">
         <v>30</v>
       </c>
@@ -1625,7 +1642,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:12" ht="20.25" customHeight="1">
+    <row r="14" spans="1:13" ht="20.25" customHeight="1">
       <c r="C14" t="s">
         <v>31</v>
       </c>
@@ -1640,7 +1657,7 @@
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:12" ht="20.25" customHeight="1">
+    <row r="15" spans="1:13" ht="20.25" customHeight="1">
       <c r="C15" t="s">
         <v>32</v>
       </c>
@@ -1654,8 +1671,11 @@
         <v>75</v>
       </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="20.25" customHeight="1">
+      <c r="M15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="20.25" customHeight="1">
       <c r="C16" t="s">
         <v>33</v>
       </c>
@@ -1667,6 +1687,9 @@
       </c>
       <c r="J16" s="5" t="s">
         <v>72</v>
+      </c>
+      <c r="M16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="3:15" ht="20.25" customHeight="1">
@@ -1702,13 +1725,13 @@
         <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="3:15" ht="20.25" customHeight="1">
@@ -1716,13 +1739,13 @@
         <v>73</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="3:15" ht="20.25" customHeight="1">
@@ -1730,13 +1753,13 @@
         <v>74</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="25" spans="3:15" ht="20.25" customHeight="1">

</xml_diff>